<commit_message>
Creación de scripts para la creación del dashboard
</commit_message>
<xml_diff>
--- a/ValidaciónCampos.xlsx
+++ b/ValidaciónCampos.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\E-learning Unigerman\Desktop\Red Centro\Carpetas de Proyectos jiji\Billy API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D2DF56C-760E-4648-B65F-AC5F5A5A0430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{242584B2-B792-4ECC-98FB-AAA20CC67512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{0A1F9E5D-558B-4070-A988-795FCB10EDCC}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Cursos" sheetId="2" r:id="rId1"/>
+    <sheet name="Inasistencias" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="79">
   <si>
     <t>Estudiante</t>
   </si>
@@ -144,6 +145,135 @@
   </si>
   <si>
     <t>Correo_electronico_personal</t>
+  </si>
+  <si>
+    <t>Cursos</t>
+  </si>
+  <si>
+    <t>[{'Codigo_modulo': 'PA', 'Nombre_modulo': 'PA - HTML – CSS ', 'Codigo_curso': 'PA01', 'Nombre_curso': 'PAE01 CHAPINERO ', 'Numero_identificacion_docente': '72167935', 'Nombre_docente': 'Polo Castro Heladio', 'Horario_curso': 'lu 7-10am', 'Periodo_curso': '2023-A', 'Fecha_inicio': '2023-02-06', 'Fecha_fin': '2023-04-09', 'Cantidad_inasistencia': 1, 'Observaciones': None, 'Inasistencias': [{'Dia': 'lunes', 'Fecha': '2023-04-03', 'Hora': '07:00 a.m. - 10:00 a.m.', 'Justificacion': False, 'Detalle_justificacion': ''}]}, {'Codigo_modulo': 'PE', 'Nombre_modulo': 'PE - JAVA SCRIPT', 'Codigo_curso': 'PE01', 'Nombre_curso': 'PAE01 CHAPINERO ', 'Numero_identificacion_docente': '72167935', 'Nombre_docente': 'Polo Castro Heladio', 'Horario_curso': 'lu 7-10am', 'Periodo_curso': '2023-A', 'Fecha_inicio': '2023-04-10', 'Fecha_fin': '2023-06-11', 'Cantidad_inasistencia': 1, 'Observaciones': None, 'Inasistencias': [{'Dia': 'lunes', 'Fecha': '2023-04-10', 'Hora': '07:00 a.m. - 10:00 a.m.', 'Justificacion': False, 'Detalle_justificacion': ''}]}]</t>
+  </si>
+  <si>
+    <t>Nombre_modulo': 'PA - HTML – CSS '</t>
+  </si>
+  <si>
+    <t>Nombre_curso': 'PAE01 CHAPINERO '</t>
+  </si>
+  <si>
+    <t>Nombre_docente': 'Polo Castro Heladio'</t>
+  </si>
+  <si>
+    <t>Cantidad_inasistencia': 1</t>
+  </si>
+  <si>
+    <t>Inasistencias': [{'Dia': 'lunes', 'Fecha': '2023-04-10', 'Hora': '07:00 a.m. - 10:00 a.m.', 'Justificacion': False, 'Detalle_justificacion': ''}]</t>
+  </si>
+  <si>
+    <t>Sede - jornada (Período)</t>
+  </si>
+  <si>
+    <t>Inicio</t>
+  </si>
+  <si>
+    <t>Finalización</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>IH Total</t>
+  </si>
+  <si>
+    <t>Cupo Máx.</t>
+  </si>
+  <si>
+    <t>N° Mat</t>
+  </si>
+  <si>
+    <t>Consecutivo</t>
+  </si>
+  <si>
+    <t>Codigo</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Nombre_docente</t>
+  </si>
+  <si>
+    <t>Cupo_maximo</t>
+  </si>
+  <si>
+    <t>Consecutivo_periodo</t>
+  </si>
+  <si>
+    <t>Nombre_periodo</t>
+  </si>
+  <si>
+    <t>Consecutivo_sede_jornada</t>
+  </si>
+  <si>
+    <t>Nombre_sede_jornada</t>
+  </si>
+  <si>
+    <t>Codigo_programa</t>
+  </si>
+  <si>
+    <t>Nombre_programa</t>
+  </si>
+  <si>
+    <t>Fecha_inicio</t>
+  </si>
+  <si>
+    <t>Fecha_fin</t>
+  </si>
+  <si>
+    <t>Cantidad_estudiantes_matriculados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JA01 </t>
+  </si>
+  <si>
+    <t>JAU01 CHAPINERO</t>
+  </si>
+  <si>
+    <t>Yency Hernandez</t>
+  </si>
+  <si>
+    <t>25.0</t>
+  </si>
+  <si>
+    <t>2023-A II</t>
+  </si>
+  <si>
+    <t>CHAPINERO - BOGOTÁ - Única</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>TÉCNICO LABORAL POR COMPETENCIAS COMO AUXILIAR EN ENFERMERÍA</t>
+  </si>
+  <si>
+    <t>2023-04-10T00:00:00-05:00</t>
+  </si>
+  <si>
+    <t>2023-06-11T00:00:00-05:00</t>
+  </si>
+  <si>
+    <t>CHAPINERO - BOGOTÁ</t>
+  </si>
+  <si>
+    <t>Conocimientos Académicos En Inglés</t>
+  </si>
+  <si>
+    <t>IAF02 CHAPINERO</t>
+  </si>
+  <si>
+    <t>Abierto</t>
+  </si>
+  <si>
+    <t>IAF02 CHAPINERO_IA - INGLÉS BÁSICO I</t>
   </si>
 </sst>
 </file>
@@ -170,7 +300,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -201,8 +331,80 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -225,16 +427,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -253,6 +463,56 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -568,11 +828,264 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{080378E9-F9AD-4868-AC16-D0E0073EAFA1}">
+  <dimension ref="A1:N10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="37" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="23">
+        <v>44837</v>
+      </c>
+      <c r="G2" s="23">
+        <v>44899</v>
+      </c>
+      <c r="H2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I2">
+        <v>100</v>
+      </c>
+      <c r="J2">
+        <v>27</v>
+      </c>
+      <c r="K2">
+        <v>25</v>
+      </c>
+      <c r="L2" t="s">
+        <v>78</v>
+      </c>
+      <c r="M2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="J4" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="K4" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="M4" s="36" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G5" t="s">
+        <v>73</v>
+      </c>
+      <c r="J5" t="s">
+        <v>67</v>
+      </c>
+      <c r="K5">
+        <v>11</v>
+      </c>
+      <c r="M5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="H9" t="s">
+        <v>57</v>
+      </c>
+      <c r="I9" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="J9" t="s">
+        <v>59</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="L9" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="M9" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="N9" s="26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>841</v>
+      </c>
+      <c r="B10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" t="s">
+        <v>67</v>
+      </c>
+      <c r="F10">
+        <v>19</v>
+      </c>
+      <c r="G10" t="s">
+        <v>68</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10" t="s">
+        <v>69</v>
+      </c>
+      <c r="J10" t="s">
+        <v>70</v>
+      </c>
+      <c r="K10" t="s">
+        <v>71</v>
+      </c>
+      <c r="L10" t="s">
+        <v>72</v>
+      </c>
+      <c r="M10" t="s">
+        <v>73</v>
+      </c>
+      <c r="N10">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20535174-3A3A-4721-8DF5-F8E59F907D75}">
   <dimension ref="A1:R8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,34 +1111,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="20" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
@@ -654,82 +1167,105 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="2">
         <v>18</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2" s="3">
         <v>44881</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="3">
+      <c r="L2" s="2">
         <v>1</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="P2" s="3">
+      <c r="P2" s="2">
         <v>1</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Q2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="R2" s="2" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="10" t="s">
         <v>7</v>
+      </c>
+      <c r="H8" t="s">
+        <v>37</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="K8" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="L8" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="M8" s="19" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>